<commit_message>
Finished changes to DfReadDataFile and updated website
Accommodates split plot design; see NEWS.md.
Unit tests updated.
Passes R CMD check in Mac; except for file size NOTE.
</commit_message>
<xml_diff>
--- a/inst/extdata/toyFiles/FROC/incorrectCaseIDsInTP.xlsx
+++ b/inst/extdata/toyFiles/FROC/incorrectCaseIDsInTP.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/toyFiles/FROC/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576AD38C-8F6F-4E4D-BB73-1CB71CC7475A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
+    <workbookView xWindow="16860" yWindow="680" windowWidth="11180" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TP" sheetId="3" r:id="rId1"/>
     <sheet name="FP" sheetId="2" r:id="rId2"/>
     <sheet name="TRUTH" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -71,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,6 +221,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -539,19 +553,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -568,7 +582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -585,7 +599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -602,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -619,7 +633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -636,7 +650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -653,7 +667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -670,7 +684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -687,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -704,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -721,7 +735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -738,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -755,7 +769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -772,7 +786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -789,7 +803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -806,7 +820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
@@ -823,7 +837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -840,7 +854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -857,7 +871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -874,7 +888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -891,7 +905,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -920,19 +934,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -946,7 +960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -960,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -974,7 +988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -988,7 +1002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1002,7 +1016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1016,7 +1030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1030,7 +1044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1044,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1072,7 +1086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1086,7 +1100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1100,7 +1114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1114,7 +1128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1128,7 +1142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1142,7 +1156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1156,7 +1170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1170,7 +1184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1210,14 +1224,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="8.83203125" style="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
@@ -1225,7 +1239,7 @@
     <col min="6" max="6" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1265,7 +1279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1285,7 +1299,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1303,7 +1317,7 @@
       </c>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>70</v>
       </c>
@@ -1321,7 +1335,7 @@
       </c>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>70</v>
       </c>
@@ -1339,7 +1353,7 @@
       </c>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>71</v>
       </c>
@@ -1357,7 +1371,7 @@
       </c>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>72</v>
       </c>
@@ -1375,7 +1389,7 @@
       </c>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>72</v>
       </c>
@@ -1393,7 +1407,7 @@
       </c>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>72</v>
       </c>
@@ -1411,7 +1425,7 @@
       </c>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>73</v>
       </c>
@@ -1429,7 +1443,7 @@
       </c>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>74</v>
       </c>
@@ -1447,7 +1461,7 @@
       </c>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1455,84 +1469,84 @@
       <c r="E13" s="2"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>

</xml_diff>